<commit_message>
split file into smaller part
</commit_message>
<xml_diff>
--- a/upload/Siuuu.xlsx
+++ b/upload/Siuuu.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Assignments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -469,12 +469,8 @@
       </c>
     </row>
     <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
   </sheetData>
-  <autoFilter ref="A1:F6"/>
+  <autoFilter ref="A1:F2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on concat videos and insert music
</commit_message>
<xml_diff>
--- a/upload/Siuuu.xlsx
+++ b/upload/Siuuu.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Assignments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -429,8 +429,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="19" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
@@ -469,11 +469,8 @@
       </c>
     </row>
     <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
   </sheetData>
-  <autoFilter ref="A1:F5"/>
+  <autoFilter ref="A1:F2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>